<commit_message>
Removes and re-adds the Excel file.
Due to an error, the Excel file was removed and then re-added.
</commit_message>
<xml_diff>
--- a/인천보고서_202512.xlsx
+++ b/인천보고서_202512.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\sidogeumgo_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A422E310-8B13-4C77-9296-57237CDD81C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8944D981-3995-42E4-A5EF-77DEDF0D7DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="상세내역" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">상세내역!$A$4:$J$75</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">상세내역!$A$1:$H$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">상세내역!$A$4:$J$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">상세내역!$A$1:$H$60</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="72">
   <si>
     <t>품질관리 상세근거</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -179,46 +179,14 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>(공통) 신년도 부서 및 사용자 신규 적용</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">⊙ 2025 보고서 개선 프로젝트 </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>보고서 개선을 위한 신규 집계 적용 및 신규 보고서 추가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(공통) 강원도 부서 정보 연계 실패 원인 분석 및 처리</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">⊙ 상반기 웹취약점 처리 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>1~31일</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>전체</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>주요 10개 항목 점검 및 처리</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>25일</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(2025.04.01~2025.04.30)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -229,15 +197,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -250,15 +209,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -271,15 +221,6 @@
     <t>18</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
@@ -287,18 +228,6 @@
   </si>
   <si>
     <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
   </si>
   <si>
     <t>29</t>
@@ -375,12 +304,83 @@
 tom.ich.fmt.xda.xSelectListICH040401By11, tom.ich.fmt.xda.xSelectListICH040401By12</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>(2025.12.01~2025.12.31)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">코어 인터페이스 변경 대응 - 회계이월, 계좌구분, 세입조정, 과오납반환 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(인천) 코어 계좌구분 변경에 따른 영향도 분석</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(인천) 코어 계좌구분 변경 대응 체크인
+KWD140202M01.xml
+crRPT041030402_2.crf
+tom.ich.rpt.xda.xSelectListICH030307By01.xml
+tom.ich.rpt.xda.xSelectOneICH030307By01.xml
+tom.ich.rpt.xda.xSelectListICH030392By01.xml
+tom.ich.rpt.xda.xSelectListICH030319By01.xml
+tom.ich.rpt.xda.xSelectListICH030320By01.xml</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(인천) 코어 회계이월 변경에 따른 영향도 분석</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(인천) 코어 회계이월 변경에 따른 기능 수정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(인천) 기금의 정기예금이월 거래 및 보통예금계좌 제외 처리 체크인
+tom.ich.rpt.xda.xSelectListICH030209By01.xml
+tom.ich.rpt.xda.xSelectListICH030324By01.xml
+tom.ich.rpt.xda.xSelectListICH030325By01.xml
+tom.ich.rpt.xda.xSelectListICH030506By01.xml</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(공통) e호조 공통코드 2026 데이터 점검</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(인천) 코어 회계이월 변경에 따른 수정 사항 체크인
+tom.ich.rpt.xda.xSelectListICH030209By01.xml
+tom.ich.rpt.xda.xSelectListICH030324By01.xml
+tom.ich.rpt.xda.xSelectListICH030325By01.xml
+tom.ich.rpt.xda.xSelectListICH030506By01.xml</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(인천) 코어 회계이월 변경에 따른 변경사항 점검</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(인천) 회계년도 변경에 따른 기초 데이터 점검</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(공통) e호조 송신 점검</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>16일</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(공통) e호조 송신 데이터 지연 원인 분석 및 처리</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -505,14 +505,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="1"/>
-      <scheme val="major"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -975,7 +967,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1107,9 +1099,6 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="58" fontId="9" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1140,9 +1129,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1164,8 +1150,41 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1221,46 +1240,10 @@
     <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1577,17 +1560,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="90" zoomScaleNormal="110" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScale="90" zoomScaleNormal="110" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" style="18" customWidth="1"/>
     <col min="2" max="2" width="82.625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="61" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.75" style="23" customWidth="1"/>
     <col min="5" max="5" width="98.625" style="18" customWidth="1"/>
     <col min="6" max="6" width="9.75" style="23" customWidth="1"/>
@@ -1597,42 +1580,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
+      <c r="A2" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="73" t="s">
+      <c r="B3" s="81"/>
+      <c r="C3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
@@ -1641,7 +1624,7 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="55" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1661,1409 +1644,1099 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="391.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="83" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="82" t="s">
+      <c r="E5" s="89"/>
+      <c r="F5" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="65"/>
+      <c r="H5" s="74"/>
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="75"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="66"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="75"/>
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="75"/>
+      <c r="A7" s="84"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="58">
+      <c r="C7" s="56">
         <v>1</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="F7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="47"/>
+      <c r="H7" s="46"/>
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
-      <c r="A8" s="75"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="58">
+        <v>43</v>
+      </c>
+      <c r="C8" s="56">
         <v>1</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="47"/>
+      <c r="H8" s="46"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="75"/>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="84"/>
       <c r="B9" s="11"/>
-      <c r="C9" s="58" t="s">
-        <v>35</v>
+      <c r="C9" s="56" t="s">
+        <v>27</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="47"/>
+      <c r="H9" s="46"/>
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="75"/>
+      <c r="A10" s="84"/>
       <c r="B10" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="58">
+        <v>43</v>
+      </c>
+      <c r="C10" s="56">
         <v>2</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="47"/>
+      <c r="H10" s="46"/>
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="75"/>
+      <c r="A11" s="84"/>
       <c r="B11" s="11"/>
-      <c r="C11" s="58" t="s">
-        <v>36</v>
+      <c r="C11" s="56" t="s">
+        <v>28</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="47"/>
+      <c r="H11" s="46"/>
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.15">
-      <c r="A12" s="75"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="58">
+        <v>43</v>
+      </c>
+      <c r="C12" s="56">
         <v>3</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="47"/>
+      <c r="H12" s="46"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="75"/>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="84"/>
       <c r="B13" s="11"/>
-      <c r="C13" s="58" t="s">
-        <v>37</v>
+      <c r="C13" s="56" t="s">
+        <v>29</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="47"/>
+      <c r="H13" s="46"/>
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="75"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="58">
+        <v>43</v>
+      </c>
+      <c r="C14" s="56">
         <v>4</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="47"/>
+      <c r="H14" s="46"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="158.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="75"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="58" t="s">
-        <v>38</v>
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="84"/>
+      <c r="B15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="56">
+        <v>5</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="56"/>
+        <v>18</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="47"/>
+      <c r="H15" s="46"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="75"/>
-      <c r="B16" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="58">
-        <v>5</v>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="47"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="56" t="s">
+        <v>30</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="47"/>
+      <c r="B17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="56">
+        <v>8</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="47"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="75"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="E17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" spans="1:8" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="47"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="47"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="75"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="58">
-        <v>6</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="E18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="30"/>
+    </row>
+    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="47"/>
+      <c r="B19" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="56">
+        <v>9</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="47"/>
-    </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="75"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="47"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="47"/>
-    </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="75"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="58">
-        <v>7</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="E20" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="30"/>
+    </row>
+    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="47"/>
+      <c r="B21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="56">
+        <v>10</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="47"/>
-    </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="48"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="E21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="30"/>
+    </row>
+    <row r="22" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="47"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="30"/>
-    </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="48"/>
-      <c r="B22" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="58">
-        <v>8</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>18</v>
-      </c>
       <c r="E22" s="11" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
       <c r="H22" s="30"/>
     </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="48"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="58" t="s">
-        <v>42</v>
+    <row r="23" spans="1:8" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.15">
+      <c r="A23" s="47"/>
+      <c r="B23" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="56">
+        <v>11</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
       <c r="H23" s="30"/>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="48"/>
+    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="47"/>
       <c r="B24" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="58">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="C24" s="56">
+        <v>12</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
       <c r="H24" s="30"/>
     </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="48"/>
+    <row r="25" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="47"/>
       <c r="B25" s="28"/>
-      <c r="C25" s="58" t="s">
-        <v>43</v>
+      <c r="C25" s="56" t="s">
+        <v>34</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="28"/>
+      <c r="E25" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="30"/>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="48"/>
-      <c r="B26" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="58">
-        <v>10</v>
+    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="47"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="56">
+        <v>15</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>69</v>
+      <c r="E26" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
       <c r="H26" s="30"/>
     </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="48"/>
+    <row r="27" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="47"/>
       <c r="B27" s="28"/>
-      <c r="C27" s="58" t="s">
-        <v>44</v>
+      <c r="C27" s="56" t="s">
+        <v>35</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="28"/>
+      <c r="E27" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
       <c r="H27" s="30"/>
     </row>
-    <row r="28" spans="1:10" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.15">
-      <c r="A28" s="48"/>
+    <row r="28" spans="1:8" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
+      <c r="A28" s="47"/>
       <c r="B28" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="58">
-        <v>11</v>
+        <v>43</v>
+      </c>
+      <c r="C28" s="56">
+        <v>16</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
       <c r="H28" s="30"/>
     </row>
-    <row r="29" spans="1:10" s="1" customFormat="1" ht="223.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="48"/>
+    <row r="29" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="47"/>
       <c r="B29" s="28"/>
-      <c r="C29" s="58" t="s">
-        <v>45</v>
+      <c r="C29" s="56" t="s">
+        <v>36</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="28"/>
+      <c r="E29" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
       <c r="H29" s="30"/>
     </row>
-    <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="48"/>
+    <row r="30" spans="1:8" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
+      <c r="A30" s="47"/>
       <c r="B30" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="58">
-        <v>12</v>
+        <v>43</v>
+      </c>
+      <c r="C30" s="56">
+        <v>17</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>74</v>
+      <c r="E30" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
       <c r="H30" s="30"/>
     </row>
-    <row r="31" spans="1:10" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="48"/>
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="47"/>
       <c r="B31" s="28"/>
-      <c r="C31" s="58" t="s">
-        <v>46</v>
+      <c r="C31" s="56" t="s">
+        <v>37</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="28"/>
+      <c r="E31" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
       <c r="H31" s="30"/>
     </row>
-    <row r="32" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="48"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="58">
-        <v>13</v>
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="82.5" x14ac:dyDescent="0.15">
+      <c r="A32" s="47"/>
+      <c r="B32" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="56">
+        <v>18</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="11"/>
+      <c r="E32" s="28" t="s">
+        <v>57</v>
+      </c>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
       <c r="H32" s="30"/>
     </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="48"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="58" t="s">
-        <v>47</v>
+    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="47"/>
+      <c r="B33" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="56">
+        <v>19</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="30"/>
     </row>
-    <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="48"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="58">
-        <v>14</v>
+    <row r="34" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="47"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="56" t="s">
+        <v>38</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="28"/>
+        <v>17</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="F34" s="29"/>
       <c r="G34" s="29"/>
       <c r="H34" s="30"/>
     </row>
-    <row r="35" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="48"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="58" t="s">
-        <v>48</v>
+    <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="47"/>
+      <c r="B35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="56">
+        <v>22</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="F35" s="29"/>
       <c r="G35" s="29"/>
       <c r="H35" s="30"/>
     </row>
-    <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="48"/>
+    <row r="36" spans="1:8" s="1" customFormat="1" ht="123.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="47"/>
       <c r="B36" s="28"/>
-      <c r="C36" s="58">
-        <v>15</v>
+      <c r="C36" s="56" t="s">
+        <v>39</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>68</v>
+        <v>17</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
       <c r="H36" s="30"/>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="48"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="28"/>
-      <c r="C37" s="58" t="s">
-        <v>49</v>
+      <c r="C37" s="56" t="s">
+        <v>40</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="28"/>
+      <c r="E37" s="28" t="s">
+        <v>65</v>
+      </c>
       <c r="F37" s="29"/>
       <c r="G37" s="29"/>
       <c r="H37" s="30"/>
     </row>
-    <row r="38" spans="1:8" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
-      <c r="A38" s="48"/>
+    <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="47"/>
       <c r="B38" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="58">
-        <v>16</v>
+        <v>43</v>
+      </c>
+      <c r="C38" s="56">
+        <v>24</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="29"/>
       <c r="H38" s="30"/>
     </row>
-    <row r="39" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="48"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="58" t="s">
-        <v>50</v>
+    <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="47"/>
+      <c r="B39" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="56">
+        <v>26</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>52</v>
+      </c>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
       <c r="H39" s="30"/>
     </row>
-    <row r="40" spans="1:8" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.15">
-      <c r="A40" s="48"/>
-      <c r="B40" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="58">
+    <row r="40" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="47"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>18</v>
-      </c>
       <c r="E40" s="28" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>
       <c r="H40" s="30"/>
     </row>
-    <row r="41" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="48"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="58" t="s">
-        <v>51</v>
+    <row r="41" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="47"/>
+      <c r="B41" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="56">
+        <v>29</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="F41" s="29"/>
       <c r="G41" s="29"/>
       <c r="H41" s="30"/>
     </row>
-    <row r="42" spans="1:8" s="1" customFormat="1" ht="82.5" x14ac:dyDescent="0.15">
-      <c r="A42" s="48"/>
-      <c r="B42" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" s="58">
-        <v>18</v>
+    <row r="42" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="47"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="56" t="s">
+        <v>42</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
       <c r="H42" s="30"/>
     </row>
-    <row r="43" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="48"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="58" t="s">
-        <v>52</v>
+    <row r="43" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="47"/>
+      <c r="B43" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="56" t="s">
+        <v>42</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
       <c r="H43" s="30"/>
     </row>
     <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="48"/>
-      <c r="B44" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="58">
-        <v>19</v>
+      <c r="A44" s="47"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="56" t="s">
+        <v>55</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>75</v>
+        <v>17</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>68</v>
       </c>
       <c r="F44" s="29"/>
       <c r="G44" s="29"/>
       <c r="H44" s="30"/>
     </row>
-    <row r="45" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="48"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="58" t="s">
-        <v>53</v>
+    <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="47"/>
+      <c r="B45" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="56" t="s">
+        <v>55</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="F45" s="29"/>
       <c r="G45" s="29"/>
       <c r="H45" s="30"/>
     </row>
-    <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="48"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="58">
+    <row r="46" spans="1:8" s="54" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="49"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="53"/>
+    </row>
+    <row r="47" spans="1:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" s="64"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="30"/>
-    </row>
-    <row r="47" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="48"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E47" s="28"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="30"/>
-    </row>
-    <row r="48" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="48"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="58">
-        <v>21</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="28"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="30"/>
-    </row>
-    <row r="49" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="48"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="28"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="30"/>
-    </row>
-    <row r="50" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="48"/>
-      <c r="B50" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="58">
-        <v>22</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="30"/>
-    </row>
-    <row r="51" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="48"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" s="28"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="30"/>
-    </row>
-    <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="48"/>
+      <c r="B47" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="25"/>
+    </row>
+    <row r="48" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="76"/>
+      <c r="B48" s="66"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="25"/>
+    </row>
+    <row r="49" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="76"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="15"/>
+    </row>
+    <row r="50" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="76"/>
+      <c r="B50" s="67"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="70"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="15"/>
+    </row>
+    <row r="51" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="76"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" s="15"/>
+    </row>
+    <row r="52" spans="1:8" s="1" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="76"/>
       <c r="B52" s="28"/>
-      <c r="C52" s="58">
-        <v>23</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E52" s="28" t="s">
-        <v>68</v>
-      </c>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="32"/>
       <c r="F52" s="29"/>
       <c r="G52" s="29"/>
-      <c r="H52" s="30"/>
-    </row>
-    <row r="53" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="48"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" s="28"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="30"/>
-    </row>
-    <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="48"/>
-      <c r="B54" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="58">
+      <c r="H52" s="33"/>
+    </row>
+    <row r="53" spans="1:8" s="40" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="F53" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="39"/>
+    </row>
+    <row r="54" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="63"/>
+      <c r="B54" s="66"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="69"/>
+      <c r="E54" s="72"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="25"/>
+    </row>
+    <row r="55" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="63"/>
+      <c r="B55" s="66"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="15"/>
+    </row>
+    <row r="56" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="63"/>
+      <c r="B56" s="67"/>
+      <c r="C56" s="70"/>
+      <c r="D56" s="70"/>
+      <c r="E56" s="73"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="15"/>
+    </row>
+    <row r="57" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="63"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="15"/>
+    </row>
+    <row r="58" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="63"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="15"/>
+    </row>
+    <row r="59" spans="1:8" s="27" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="64"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="43"/>
+    </row>
+    <row r="60" spans="1:8" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="30"/>
-    </row>
-    <row r="55" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="48"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E55" s="28"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="30"/>
-    </row>
-    <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="48"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="58">
-        <v>25</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="28"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="30"/>
-    </row>
-    <row r="57" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="48"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" s="28"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="30"/>
-    </row>
-    <row r="58" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="48"/>
-      <c r="B58" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="58">
-        <v>26</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="30"/>
-    </row>
-    <row r="59" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="48"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E59" s="28"/>
-      <c r="F59" s="29"/>
-      <c r="G59" s="29"/>
-      <c r="H59" s="30"/>
-    </row>
-    <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="48"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="58">
-        <v>27</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" s="28"/>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="30"/>
-    </row>
-    <row r="61" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="48"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E61" s="28"/>
-      <c r="F61" s="29"/>
-      <c r="G61" s="29"/>
-      <c r="H61" s="30"/>
-    </row>
-    <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="48"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="58">
-        <v>28</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E62" s="28"/>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="30"/>
-    </row>
-    <row r="63" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="48"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63" s="28"/>
-      <c r="F63" s="29"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="30"/>
-    </row>
-    <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="48"/>
-      <c r="B64" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C64" s="58">
-        <v>29</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="F64" s="29"/>
-      <c r="G64" s="29"/>
-      <c r="H64" s="30"/>
-    </row>
-    <row r="65" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="48"/>
-      <c r="B65" s="28"/>
-      <c r="C65" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E65" s="28"/>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="30"/>
-    </row>
-    <row r="66" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="48"/>
-      <c r="B66" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="F66" s="29"/>
-      <c r="G66" s="29"/>
-      <c r="H66" s="30"/>
-    </row>
-    <row r="67" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="48"/>
-      <c r="B67" s="28"/>
-      <c r="C67" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E67" s="28"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29"/>
-      <c r="H67" s="30"/>
-    </row>
-    <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="48"/>
-      <c r="B68" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="30"/>
-    </row>
-    <row r="69" spans="1:8" s="55" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="50"/>
-      <c r="B69" s="51"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="52"/>
-      <c r="E69" s="51"/>
-      <c r="F69" s="53"/>
-      <c r="G69" s="53"/>
-      <c r="H69" s="54"/>
-    </row>
-    <row r="70" spans="1:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="B70" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="C70" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="D70" s="86" t="s">
-        <v>14</v>
-      </c>
-      <c r="E70" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="F70" s="24" t="s">
+      <c r="E60" s="31"/>
+      <c r="F60" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G70" s="24" t="s">
+      <c r="G60" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="H70" s="25"/>
-    </row>
-    <row r="71" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="67"/>
-      <c r="B71" s="88"/>
-      <c r="C71" s="84"/>
-      <c r="D71" s="84"/>
-      <c r="E71" s="88"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="25"/>
-    </row>
-    <row r="72" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="67"/>
-      <c r="B72" s="88"/>
-      <c r="C72" s="84"/>
-      <c r="D72" s="84"/>
-      <c r="E72" s="88"/>
-      <c r="F72" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G72" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H72" s="15"/>
-    </row>
-    <row r="73" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="67"/>
-      <c r="B73" s="89"/>
-      <c r="C73" s="85"/>
-      <c r="D73" s="85"/>
-      <c r="E73" s="89"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
-      <c r="H73" s="15"/>
-    </row>
-    <row r="74" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="67"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G74" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H74" s="15"/>
-    </row>
-    <row r="75" spans="1:8" s="1" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="67"/>
-      <c r="B75" s="28"/>
-      <c r="C75" s="49"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="29"/>
-      <c r="G75" s="29"/>
-      <c r="H75" s="33"/>
-    </row>
-    <row r="76" spans="1:8" s="40" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="90" t="s">
-        <v>21</v>
-      </c>
-      <c r="B76" s="93" t="s">
-        <v>26</v>
-      </c>
-      <c r="C76" s="83" t="s">
-        <v>30</v>
-      </c>
-      <c r="D76" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="E76" s="94" t="s">
-        <v>27</v>
-      </c>
-      <c r="F76" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="G76" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="H76" s="39"/>
-    </row>
-    <row r="77" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="91"/>
-      <c r="B77" s="88"/>
-      <c r="C77" s="84"/>
-      <c r="D77" s="84"/>
-      <c r="E77" s="95"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="24"/>
-      <c r="H77" s="25"/>
-    </row>
-    <row r="78" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="91"/>
-      <c r="B78" s="88"/>
-      <c r="C78" s="84"/>
-      <c r="D78" s="84"/>
-      <c r="E78" s="95"/>
-      <c r="F78" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G78" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H78" s="15"/>
-    </row>
-    <row r="79" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="91"/>
-      <c r="B79" s="89"/>
-      <c r="C79" s="85"/>
-      <c r="D79" s="85"/>
-      <c r="E79" s="96"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="15"/>
-    </row>
-    <row r="80" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="91"/>
-      <c r="B80" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C80" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D80" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E80" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F80" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G80" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H80" s="15"/>
-    </row>
-    <row r="81" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="91"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="16"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="15"/>
-    </row>
-    <row r="82" spans="1:8" s="27" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="92"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="41"/>
-      <c r="D82" s="41"/>
-      <c r="E82" s="42"/>
-      <c r="F82" s="26"/>
-      <c r="G82" s="26"/>
-      <c r="H82" s="43"/>
-    </row>
-    <row r="83" spans="1:8" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B83" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C83" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="D83" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="E83" s="31"/>
-      <c r="F83" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="G83" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="H83" s="37"/>
-    </row>
-    <row r="84" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="C84" s="60"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B85" s="1"/>
-      <c r="C85" s="61"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="20"/>
-      <c r="G85" s="20"/>
-      <c r="H85" s="21"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B86" s="1"/>
-      <c r="C86" s="62"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="20"/>
-      <c r="G86" s="20"/>
-      <c r="H86" s="21"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B87" s="1"/>
-      <c r="C87" s="62"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="20"/>
-      <c r="G87" s="20"/>
-      <c r="H87" s="21"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B88" s="1"/>
-      <c r="C88" s="62"/>
-      <c r="D88" s="20"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="20"/>
-      <c r="G88" s="20"/>
-      <c r="H88" s="21"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B89" s="1"/>
-      <c r="C89" s="62"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="20"/>
-      <c r="H89" s="21"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B90" s="1"/>
-      <c r="C90" s="62"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="22"/>
-      <c r="F90" s="20"/>
-      <c r="G90" s="20"/>
-      <c r="H90" s="21"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B91" s="1"/>
-      <c r="C91" s="62"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="22"/>
-      <c r="F91" s="20"/>
-      <c r="G91" s="20"/>
-      <c r="H91" s="21"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B92" s="1"/>
-      <c r="C92" s="62"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="20"/>
-      <c r="G92" s="20"/>
-      <c r="H92" s="21"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B93" s="1"/>
-      <c r="C93" s="62"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="22"/>
-      <c r="F93" s="20"/>
-      <c r="G93" s="20"/>
-      <c r="H93" s="21"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B94" s="1"/>
-      <c r="C94" s="62"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="20"/>
-      <c r="G94" s="20"/>
-      <c r="H94" s="21"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B95" s="1"/>
-      <c r="C95" s="62"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="22"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="20"/>
-      <c r="H95" s="21"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B96" s="1"/>
-      <c r="C96" s="62"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="22"/>
-      <c r="F96" s="20"/>
-      <c r="G96" s="20"/>
-      <c r="H96" s="21"/>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B97" s="1"/>
-      <c r="C97" s="62"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="22"/>
-      <c r="F97" s="20"/>
-      <c r="G97" s="20"/>
-      <c r="H97" s="21"/>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B98" s="1"/>
-      <c r="C98" s="62"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="22"/>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B99" s="1"/>
-      <c r="C99" s="62"/>
-      <c r="D99" s="20"/>
-      <c r="E99" s="22"/>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B100" s="1"/>
-      <c r="C100" s="62"/>
-      <c r="D100" s="20"/>
-      <c r="E100" s="22"/>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B101" s="1"/>
-      <c r="C101" s="62"/>
-      <c r="D101" s="20"/>
-      <c r="E101" s="22"/>
+      <c r="H60" s="37"/>
+    </row>
+    <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C61" s="58"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="21"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
+      <c r="C63" s="60"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="21"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+      <c r="C64" s="60"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="21"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="21"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="21"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
+      <c r="C67" s="60"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="21"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B68" s="1"/>
+      <c r="C68" s="60"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="21"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B69" s="1"/>
+      <c r="C69" s="60"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="21"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B70" s="1"/>
+      <c r="C70" s="60"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="21"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B71" s="1"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="21"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B72" s="1"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="21"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+      <c r="C73" s="60"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="21"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+      <c r="C74" s="60"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="21"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+      <c r="C75" s="60"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="22"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+      <c r="C76" s="60"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="22"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+      <c r="C77" s="60"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="22"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+      <c r="C78" s="60"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="A47:A52"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A5:A20"/>
+    <mergeCell ref="A5:A15"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="E53:E56"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.3" right="0" top="0.3" bottom="0.11811023622047245" header="0.22" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="26" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="48" max="7" man="1"/>
-    <brk id="82" max="7" man="1"/>
+    <brk id="33" max="7" man="1"/>
+    <brk id="59" max="7" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>